<commit_message>
Criação dos botões do menu
</commit_message>
<xml_diff>
--- a/Aquabox_pico/Hardware/Identificacao_GPIOs.xlsx
+++ b/Aquabox_pico/Hardware/Identificacao_GPIOs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioGit\Embarcatech\Aquabox_pico\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034B0B50-C95C-45F0-A85E-863423DC581E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A3A5CA-17CE-40B5-97A4-6841F4222296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{088BD24A-FF7C-422D-AD8A-3645227017AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -124,6 +124,30 @@
   </si>
   <si>
     <t>Sensor de nível alto instalado na caixa d'água</t>
+  </si>
+  <si>
+    <t>Pushbutton vermelho</t>
+  </si>
+  <si>
+    <t>Pushbutton verde</t>
+  </si>
+  <si>
+    <t>Pushbutton amarelo</t>
+  </si>
+  <si>
+    <t>Pushbutton azul</t>
+  </si>
+  <si>
+    <t>Botão para seleção no menu de opções</t>
+  </si>
+  <si>
+    <t>Botão para retornar a tela inicial do relógio</t>
+  </si>
+  <si>
+    <t>Botão para seleção de subitem do menu de opções</t>
+  </si>
+  <si>
+    <t>Botão para entrada de dados de configuração</t>
   </si>
 </sst>
 </file>
@@ -536,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FFF972-9E47-489F-99F1-A699774A2337}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,14 +788,70 @@
       <c r="A17" s="3">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="3">
         <v>19</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5">
+        <v>8</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>16</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3">
+        <v>9</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="5">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="3">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>